<commit_message>
formatting changes to excel outputs, include filenames tab in Program_Diff export
</commit_message>
<xml_diff>
--- a/comparison/output/SEACARQAQCFlagCode_Overview.xlsx
+++ b/comparison/output/SEACARQAQCFlagCode_Overview.xlsx
@@ -532,6 +532,17 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="41.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="13.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="18.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="4.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="4.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="4.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="7.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">

</xml_diff>